<commit_message>
Cập Nhật Bảng Tham Số
</commit_message>
<xml_diff>
--- a/ThamSo.xlsx
+++ b/ThamSo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minhd\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637D5FDC-34D5-423B-90D0-FE2743BFB364}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822307C2-BE58-4AED-9753-68A9CF958154}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>d(i)</t>
   </si>
   <si>
-    <t>m = Tỷ Lệ Tử Vong</t>
-  </si>
-  <si>
     <t>a = Tỷ Lệ Tiến Cấp</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>P(s) = Tỷ Lệ Sống Sót Nhưng Không Chuyển Giai Đoạn</t>
+  </si>
+  <si>
+    <t>m = Tỷ Lệ Tử Vong Từng Giai Đoàn</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,19 +442,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>

</xml_diff>